<commit_message>
Fix KeyError in portfolio mapping column name handling
</commit_message>
<xml_diff>
--- a/data/references/Portfolio Mapping/PEMI_Account_name_porfolio_mapping.xlsx
+++ b/data/references/Portfolio Mapping/PEMI_Account_name_porfolio_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserProfile\Documents\@ VFC\@ VFC-DATA\PEMI Report Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserProfile\Documents\@ VFC\pemi-automation\trial-balance\data\references\Portfolio Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E0D1179-2DF3-4F3D-B514-811C1BB9613A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9357A91F-4BBD-4988-99A5-A3766448D17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4243C91C-0AEE-42DD-9EB1-058807637C26}"/>
+    <workbookView xWindow="1920" yWindow="-14280" windowWidth="21600" windowHeight="11235" xr2:uid="{4243C91C-0AEE-42DD-9EB1-058807637C26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Philequity Alpha One Fund, Inc.</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t xml:space="preserve">Philequity MSCI Philippines Index Fund, Inc.	</t>
+  </si>
+  <si>
+    <t>Fund_Code</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +526,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>